<commit_message>
Saved some raw spectra as unmodified txt files. Updated progress spreadsheet
</commit_message>
<xml_diff>
--- a/Data/SampleProgress.xlsx
+++ b/Data/SampleProgress.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Control</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>(temp/10)_time_1(2)</t>
+  </si>
+  <si>
+    <t>AFM</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,6 +425,36 @@
       <c r="A2">
         <v>100</v>
       </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
       <c r="M2" t="s">
         <v>4</v>
       </c>
@@ -429,6 +462,15 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>